<commit_message>
prepare base simulation plots exp22
</commit_message>
<xml_diff>
--- a/output/exp14_hyperparam_tuning/stats_duration.xlsx
+++ b/output/exp14_hyperparam_tuning/stats_duration.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I844141\Documents\Unisinos\2019-2\TCCII\workspace\TCC-II\output\exp14_hyperparam_tuning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AB2E904-DEDB-4255-A0AA-E7BAE73BE0D3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB3DC9F-B52E-4105-97AF-10727BE8842A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stats_duration" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
   <si>
     <t>exp1</t>
   </si>
@@ -35,9 +36,6 @@
   </si>
   <si>
     <t>aggregated</t>
-  </si>
-  <si>
-    <t>prefix</t>
   </si>
   <si>
     <t>mean</t>
@@ -66,11 +64,17 @@
   <si>
     <t>rf_avg_veh_number_0.1_0.7_0.6</t>
   </si>
+  <si>
+    <t>learning rate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0E+00"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -548,9 +552,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -596,7 +602,13 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -918,11 +930,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -956,72 +968,72 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
       <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>7</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
-        <v>9</v>
-      </c>
       <c r="N2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="R2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>269.89723818869999</v>
@@ -1086,7 +1098,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>261.45927379784098</v>
@@ -1151,7 +1163,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>255.603462778634</v>
@@ -1216,7 +1228,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>267.86092808075102</v>
@@ -1281,7 +1293,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>264.74512827702199</v>
@@ -1346,11 +1358,193 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:U7">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>B3=MIN(B$3:B$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D171B7E-2629-4B32-85B3-346E9DC726C8}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="B3" s="3">
+        <v>261.61152390298599</v>
+      </c>
+      <c r="C3" s="3">
+        <v>167.174671233715</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1294</v>
+      </c>
+      <c r="E3" s="3">
+        <v>254.53037319316201</v>
+      </c>
+      <c r="F3" s="3">
+        <v>136.82626172803299</v>
+      </c>
+      <c r="G3">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>271.06161502873903</v>
+      </c>
+      <c r="C4" s="3">
+        <v>174.43005880489301</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1164</v>
+      </c>
+      <c r="E4" s="3">
+        <v>250.00074445818299</v>
+      </c>
+      <c r="F4" s="3">
+        <v>120.413517771977</v>
+      </c>
+      <c r="G4">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>257.49130800504599</v>
+      </c>
+      <c r="C5" s="3">
+        <v>153.41869598962899</v>
+      </c>
+      <c r="D5" s="3">
+        <v>981</v>
+      </c>
+      <c r="E5" s="3">
+        <v>247.05411828070899</v>
+      </c>
+      <c r="F5" s="3">
+        <v>118.537611698541</v>
+      </c>
+      <c r="G5">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="B6" s="3">
+        <v>272.38553203420702</v>
+      </c>
+      <c r="C6" s="3">
+        <v>180.700757989214</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1081</v>
+      </c>
+      <c r="E6" s="3">
+        <v>253.317696795518</v>
+      </c>
+      <c r="F6" s="3">
+        <v>123.559904090088</v>
+      </c>
+      <c r="G6">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>257.50995373615501</v>
+      </c>
+      <c r="C7" s="3">
+        <v>160.60208332507301</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1072</v>
+      </c>
+      <c r="E7" s="3">
+        <v>249.091008815511</v>
+      </c>
+      <c r="F7" s="3">
+        <v>121.18722451017599</v>
+      </c>
+      <c r="G7">
+        <v>981.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B3:F7">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>B3=MIN(B$3:B$7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G7">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>G3=MIN(G$3:G$7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>